<commit_message>
update validasi import data pengguna
</commit_message>
<xml_diff>
--- a/public/template_excel/template_export_level_mahasiswa.xlsx
+++ b/public/template_excel/template_export_level_mahasiswa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8fc1a9f9b85c3689/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3A1FC87-60CB-4223-B3B3-6D92FCA5B707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{E3A1FC87-60CB-4223-B3B3-6D92FCA5B707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{673F0F39-B6E7-451B-9952-157CB0415E87}"/>
   <bookViews>
-    <workbookView xWindow="12120" yWindow="2340" windowWidth="12510" windowHeight="11430" xr2:uid="{4DC91AB0-04AB-49F1-A83B-FD6BE91D8838}"/>
+    <workbookView xWindow="10665" yWindow="1755" windowWidth="12510" windowHeight="11430" xr2:uid="{4DC91AB0-04AB-49F1-A83B-FD6BE91D8838}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,23 +42,29 @@
     <t>nim</t>
   </si>
   <si>
-    <t>program_studi_id</t>
-  </si>
-  <si>
     <t>angkatan</t>
   </si>
   <si>
     <t>status</t>
   </si>
+  <si>
+    <t>kode_program_studi</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,6 +107,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -403,12 +413,12 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -420,16 +430,17 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>